<commit_message>
implemented Axe in screens
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_PM_APFA_DebtInvestmentProfile_Regression_001.xlsx
+++ b/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_PM_APFA_DebtInvestmentProfile_Regression_001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\MStars_Automation\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdighe\Documents\MDOT\rstars\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B484E91-3794-4E14-BC37-D928DDAA6DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056278FD-F791-4302-A38E-5C03F3B401A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{397F6C8C-76D5-4724-9027-584DB73AF3FC}"/>
   </bookViews>
@@ -108,16 +108,16 @@
     <t>Open next profile</t>
   </si>
   <si>
-    <t>TC_PR_APFA_DebtInvestmentProfile_ListView</t>
-  </si>
-  <si>
-    <t>TC_PR_APFA_DebtInvestmentProfile_AddNewProfile</t>
-  </si>
-  <si>
-    <t>TC_PR_APFA_DebtInvestmentProfile_EditProfile</t>
-  </si>
-  <si>
-    <t>TC_PR_APFA_DebtInvestmentProfile_DeleteProfile</t>
+    <t>TC_PM_APFA_DebtInvestmentProfile_AddNewProfile</t>
+  </si>
+  <si>
+    <t>TC_PM_APFA_DebtInvestmentProfile_EditProfile</t>
+  </si>
+  <si>
+    <t>TC_PM_APFA_DebtInvestmentProfile_DeleteProfile</t>
+  </si>
+  <si>
+    <t>TC_PM_APFA_ListView_D2</t>
   </si>
 </sst>
 </file>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A1E7EF-77D3-41B3-8B98-2D4334A55173}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,7 +649,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -669,7 +669,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
@@ -709,7 +709,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
@@ -769,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>21</v>

</xml_diff>